<commit_message>
Ready to collect data
Tables are set. floor_type the only one I will let as string, probably after it will be set. Last the furnished column done.
</commit_message>
<xml_diff>
--- a/documentation/database_overview.xlsx
+++ b/documentation/database_overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCRIPTS\immoDATA\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EA8E64-3664-443E-83A4-BFCF7FBEFB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58508F5C-7284-497C-A4C4-CC509125DDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="overview" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -179,6 +178,48 @@
   </si>
   <si>
     <t>VARCHAR (150)</t>
+  </si>
+  <si>
+    <t>washing_machine</t>
+  </si>
+  <si>
+    <t>dishwasher</t>
+  </si>
+  <si>
+    <t>garden</t>
+  </si>
+  <si>
+    <t>pets</t>
+  </si>
+  <si>
+    <t>balcony</t>
+  </si>
+  <si>
+    <t>terrace</t>
+  </si>
+  <si>
+    <t>garage</t>
+  </si>
+  <si>
+    <t>elevator</t>
+  </si>
+  <si>
+    <t>VARCHAR (100)</t>
+  </si>
+  <si>
+    <t>id_heating</t>
+  </si>
+  <si>
+    <t>bathtub</t>
+  </si>
+  <si>
+    <t>shower</t>
+  </si>
+  <si>
+    <t>guest_wc</t>
+  </si>
+  <si>
+    <t>furnished</t>
   </si>
 </sst>
 </file>
@@ -202,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +286,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -273,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -283,6 +348,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +678,7 @@
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -887,225 +956,246 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="E17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="E19" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="10"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="10"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="10"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="10"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="10"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="C30" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="C32" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="C33" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B34" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>7</v>
@@ -1113,119 +1203,208 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="12"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B54" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="C54" s="10"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+      <c r="C56" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B57" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="C57" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B58" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="C58" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B59" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="C59" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B60" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C60" s="8" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>